<commit_message>
updated the interview guide
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="interview Guide" sheetId="1" r:id="rId1"/>
+    <sheet name="wait List" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -805,4 +806,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>